<commit_message>
Updated Validation Set dataset
</commit_message>
<xml_diff>
--- a/Validation set.xlsx
+++ b/Validation set.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_CNR\Climate Change - Cetacean Abundance Studies\Nuovo DATASET ESPERIMENTI\0_Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\1_Environmental variables and machine learning models to predict cetacean abundance in the Central-eastern Mediterranean Sea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5C2791-2EEC-49CC-8CBA-C670C948530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA280F2A-63FA-4EE3-B58F-174408731149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4DE38B3C-2B8C-41B8-AF9B-1637EC625F19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE38B3C-2B8C-41B8-AF9B-1637EC625F19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Original dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="original dataset" sheetId="1" r:id="rId1"/>
     <sheet name="dataset used for testing ML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="chl" localSheetId="0">'Original dataset'!$CE$2:$CL$8</definedName>
-    <definedName name="chl_sat" localSheetId="0">'Original dataset'!$CM$2:$CM$8</definedName>
-    <definedName name="DENS" localSheetId="0">'Original dataset'!$Z$2:$AG$8</definedName>
-    <definedName name="distance" localSheetId="0">'Original dataset'!$G$1:$G$8</definedName>
-    <definedName name="maxDepth" localSheetId="0">'Original dataset'!$I$2:$I$8</definedName>
-    <definedName name="maxDepth_emodnet_valid" localSheetId="0">'Original dataset'!$H$2:$H$8</definedName>
-    <definedName name="mlotst" localSheetId="0">'Original dataset'!$AH$2:$AH$8</definedName>
-    <definedName name="N2_cyH" localSheetId="0">'Original dataset'!$CN$2:$CT$8</definedName>
-    <definedName name="no3_" localSheetId="0">'Original dataset'!#REF!</definedName>
-    <definedName name="no3_1" localSheetId="0">'Original dataset'!$BG$2:$BN$8</definedName>
-    <definedName name="nppv" localSheetId="0">'Original dataset'!$AY$2:$BF$8</definedName>
-    <definedName name="phyc" localSheetId="0">'Original dataset'!$BW$2:$CD$8</definedName>
-    <definedName name="po4_" localSheetId="0">'Original dataset'!#REF!</definedName>
-    <definedName name="po4_1" localSheetId="0">'Original dataset'!$BO$2:$BV$8</definedName>
-    <definedName name="so" localSheetId="0">'Original dataset'!$R$2:$Y$8</definedName>
-    <definedName name="thetao" localSheetId="0">'Original dataset'!$J$2:$Q$8</definedName>
-    <definedName name="VEL_dir_2" localSheetId="0">'Original dataset'!$AQ$2:$AX$8</definedName>
-    <definedName name="VEL_module" localSheetId="0">'Original dataset'!$AI$2:$AP$8</definedName>
+    <definedName name="chl" localSheetId="0">'original dataset'!$CE$2:$CL$8</definedName>
+    <definedName name="chl_sat" localSheetId="0">'original dataset'!$CM$2:$CM$8</definedName>
+    <definedName name="DENS" localSheetId="0">'original dataset'!$Z$2:$AG$8</definedName>
+    <definedName name="distance" localSheetId="0">'original dataset'!$G$1:$G$8</definedName>
+    <definedName name="maxDepth" localSheetId="0">'original dataset'!$I$2:$I$8</definedName>
+    <definedName name="maxDepth_emodnet_valid" localSheetId="0">'original dataset'!$H$2:$H$8</definedName>
+    <definedName name="mlotst" localSheetId="0">'original dataset'!$AH$2:$AH$8</definedName>
+    <definedName name="N2_cyH" localSheetId="0">'original dataset'!$CN$2:$CT$8</definedName>
+    <definedName name="no3_" localSheetId="0">'original dataset'!#REF!</definedName>
+    <definedName name="no3_1" localSheetId="0">'original dataset'!$BG$2:$BN$8</definedName>
+    <definedName name="nppv" localSheetId="0">'original dataset'!$AY$2:$BF$8</definedName>
+    <definedName name="phyc" localSheetId="0">'original dataset'!$BW$2:$CD$8</definedName>
+    <definedName name="po4_" localSheetId="0">'original dataset'!#REF!</definedName>
+    <definedName name="po4_1" localSheetId="0">'original dataset'!$BO$2:$BV$8</definedName>
+    <definedName name="so" localSheetId="0">'original dataset'!$R$2:$Y$8</definedName>
+    <definedName name="thetao" localSheetId="0">'original dataset'!$J$2:$Q$8</definedName>
+    <definedName name="VEL_dir_2" localSheetId="0">'original dataset'!$AQ$2:$AX$8</definedName>
+    <definedName name="VEL_module" localSheetId="0">'original dataset'!$AI$2:$AP$8</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1128,23 +1128,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="thetao" connectionId="14" xr16:uid="{C3C51702-524B-5B42-B3CA-9A3759E70366}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="mlotst" connectionId="7" xr16:uid="{D578EC51-2F11-F54E-8179-933757C91F9B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="mlotst" connectionId="7" xr16:uid="{D578EC51-2F11-F54E-8179-933757C91F9B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="po4_1" connectionId="12" xr16:uid="{84C6D228-841E-504C-9390-1465C717ECA3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="maxDepth_emodnet_valid" connectionId="6" xr16:uid="{AD3ACFC5-1591-8D4A-A5D6-70E9DD96719B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="nppv" connectionId="10" xr16:uid="{B47B1461-D6A7-0143-BBFD-810F383A3A97}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="N2_cyH" connectionId="8" xr16:uid="{75C1F554-AC88-154A-B44E-4A2AC600562B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DENS" connectionId="3" xr16:uid="{250ACD58-78C1-2646-8BE3-C275B705379C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DENS" connectionId="3" xr16:uid="{250ACD58-78C1-2646-8BE3-C275B705379C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="chl_sat" connectionId="2" xr16:uid="{11282423-372D-1742-8AE4-FC63113ABCB1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1152,43 +1152,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="phyc" connectionId="11" xr16:uid="{C784D22F-06F0-0942-941E-AD044F6FC342}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="so" connectionId="13" xr16:uid="{7835D85A-E471-5447-B7E0-BCB21CAB0276}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="maxDepth" connectionId="5" xr16:uid="{13742355-426C-6E41-99C4-503B4F006607}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="no3_1" connectionId="9" xr16:uid="{3B173723-B194-AF42-BF4E-DB949CF43264}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="maxDepth_emodnet_valid" connectionId="6" xr16:uid="{AD3ACFC5-1591-8D4A-A5D6-70E9DD96719B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="VEL_module" connectionId="16" xr16:uid="{EC76085C-6291-994A-BF63-E68F4204BBE3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="thetao" connectionId="14" xr16:uid="{C3C51702-524B-5B42-B3CA-9A3759E70366}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="distance" connectionId="4" xr16:uid="{BBD3D763-2248-FA4D-A087-251A0FB34EE9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="chl" connectionId="1" xr16:uid="{FC93706E-BEC1-6F41-9BD6-9F3416F8A570}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="nppv" connectionId="10" xr16:uid="{B47B1461-D6A7-0143-BBFD-810F383A3A97}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="so" connectionId="13" xr16:uid="{7835D85A-E471-5447-B7E0-BCB21CAB0276}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="no3_1" connectionId="9" xr16:uid="{3B173723-B194-AF42-BF4E-DB949CF43264}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="VEL_module" connectionId="16" xr16:uid="{EC76085C-6291-994A-BF63-E68F4204BBE3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="po4_1" connectionId="12" xr16:uid="{84C6D228-841E-504C-9390-1465C717ECA3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="chl_sat" connectionId="2" xr16:uid="{11282423-372D-1742-8AE4-FC63113ABCB1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="phyc" connectionId="11" xr16:uid="{C784D22F-06F0-0942-941E-AD044F6FC342}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="N2_cyH" connectionId="8" xr16:uid="{75C1F554-AC88-154A-B44E-4A2AC600562B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1490,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE3B970-48BC-4A28-BF59-6847FB8EDB85}">
   <dimension ref="A1:CT8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3930,7 +3930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8884220-2830-024F-980F-5EAFEA21D8BA}">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>

</xml_diff>